<commit_message>
Several features added. - Distraction logging added, such that when focusing. Distractions can be logged to allow user to focus on task and review distraction later.
- Changed "database" to an google sheets utilizing
Google sheets services. Allowing for better cloud integration with my data.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="52" workbookViewId="0">
       <selection activeCell="C19" sqref="A19:XFD19"/>
@@ -2443,7 +2443,1481 @@
 Overall the code was quite simple to read, it was initialization code, obviously I don't understand it all. But I made progres.</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-12-16 13:47:49</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>brain storm how to deal with stm32. 
+What exactly are we going to be doing today.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>8.57</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>10.21</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Starting to get distracted and tired. We were able
+to identify what tasks to do for today. though so lets call it quits
+and just move on.
+Eyes are quite tired today. Had a nice little rest there.
+Thought a bit about the database, seems that it may need to be a bit more complicated, but that is okay in order for it to work, since we 
+have such cascaded goals. We will need to reduce some redundancies
+within the database.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-12-16 14:17:15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Creating the algorithm, to turn on an LED via the LP5812.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>30.28</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>45.04</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Interesting, after contemplation, I felt the need to REDO
+a new canvas. Even though a meta goal was created.
+As we wanted a fresh mind. It seems we are in problem
+solving mode. So we enter into one of the blocks.
+So fucking tired man.
+Starting to get a bit tired. Once again, not sure if I will 
+recover this time.
+Hit some pretty good milestones though, breaking the problem down
+is quite nice.
+I feel like taking a break, so I will. After 30 mins of studying. 
+Listened to some audio book.
+True to yourself, do shoot the bow without shoooting the bow. 
+Let all distinctions and judgements dissolve. Be in the present moment.
+Also stimultaneously rested my eyes.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-12-16 15:37:37</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Creating the algorithm, to turn on an LED via the LP5812.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>31.03</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>stm32, doesn't work. 
+This seems like such a tall tower to climb, doesn't seem like a good idea to execute upon this.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-12-16 17:24:17</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>MEDITATE</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>60.01</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>11.70</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>3.55</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Had little moments of present momentness, however just briefly.
+THen WHOOP. Popped back into my standard reallity. My default mindstate. Numb to everything. 
+Just running your default pathways. Let go of the default, defuse your thoughts in your mind. Let go of all judgements, you do not know anything.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-12-17 11:24:20</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Do research on LP5812, specifically the registers in the beginning.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>5.01</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2.38</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-12-17 11:31:47</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Do research on LP5812, specifically the registers in the beginning.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>4.60</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-12-17 12:19:43</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Do research on LP5812, specifically the registers in the beginning.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>50.01</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>7.67</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Yeah, about 3 long distractions. Very long. Probably half the time was distracted.
+Anyways, lets back t o it.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-12-17 13:13:08</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Do research on LP5812, specifically the registers in the beginning.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>50.01</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>21.89</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>52.07</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>how do inductors create magnetic fields
+How do capacitors create electric fields.
+Overtimmed, got distracted, and decided this is it. 
+Failure, acceptance and love of failure is why i'm able to do this which is so counter-intuitive. 
+Something within me is popping up,  it is really really dark. Really dark.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-12-17 16:41:09</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>MEDITATION</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>60.01</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>29.77</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-12-17 17:52:28</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>See if Device address is truley responding</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>8.90</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>29.77</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>3.34</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Device address has been verified to respond to address.
+Device address has been verified to not respond to 0x00</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-12-17 18:05:03</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Learn how the I2C for this device works. Do we really need to use another function</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>8.65</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>29.77</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>16.41</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So basically, 5 bits for device address, alongside 10 bits for address.
+WRITE COMMAND
+1. Communicate device address.
+2. +2 MSB
+3. Acknowledge + 0, which is the write bit
+4. Transmit the rest of the REGISTER ADDRESSES + write bit
+READ COMMAND:
+1. Start condition + device address + write
+2. Register address + read
+3. Restart
+4. Register write address
+5. Read the byte of data.
+6. Acknowledge if you want to continue receiving more data.
+or Not acknowledge if you want to stop receiving data.
+7. Finally we have the stop condition.
+Visualization for I2C is like a swimmer doing the dolphin kick. The timer starts, aka is high. Falling edge. As soon as the timer starts. BOOM the dolphin or swimmer jumps into the water. doing dolphin kicks.
+Until the stop condition where the swimmer gets back up from underneath the water where he is a rising edge now. Where he heads up to the surface indicating the high clock signal.
+Repeat start: is simply jumping back to the start, redoing it without ending. Like going back in time to restart.
+Not acknowledge is when the you have communicated with the app, I have had enough. After every swim cycle lap you can either get up and say stop. Or you can acknowledge with your coach going like "thumbs up" 
+Continue on swimming. Or If you are now listening to your coach speaking and eventually you go like eh not ecknowledge hands down. No more hands up and he stops talking.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-12-17 18:56:13</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Implementation of the initialization of the PROGRAM.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>24.67</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>29.77</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>37.09</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-12-18 15:26:13</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Create READ, and WRITE LP5812 I2C functions
+</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>50.01</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>12.85</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>5.12</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Ended up doing some random shit. Kinda weird.
+Like learning how pointers work in more depth as there was
+some stuff I didn't quite understand within 
+the HAL I2C functions.
+postman analogy.
+An array is a pointer to the address of first element.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-12-18 16:39:49</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Test LP5812 I2C read and write</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>32.74</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>12.85</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2.68</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>TBH, I'm going to assume it works, it seems that so far 
+we have no reason to believe it will not work.
+One question I have is what is that testing for configuration error.
+How do you even get one.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-12-18 17:20:21</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VERIFY AND FINALIZE
+INITIALIZATION CODE. </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>7.50</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>12.85</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Task too big, going to go smaller.
+Distrated for a bit.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-12-18 17:28:13</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>UPload algorithm onto NOTION and plan.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>16.59</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>12.85</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>68.39</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Did upload it onto notion. I just went through the datasheet, and there's some things we need to verify. But yeah.
+Like ther's a chance that my led's have 3.6V max. which I only have 3.3V, but we'll drive it at 3.3V anyways. Cuz that's what we got.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-12-18 18:58:18</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MEDITATE</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>22.47</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>12.85</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Others harming you is not other harming you, it's you harming you. 
+Take responsibiltiy for this..
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-12-18 19:21:35</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>MEDITATE</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>12.85</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Meditation is not about controlling your thoughts, but detaching yourself and going above your thoughts. Seeing thoughts as thoughts, not as reality.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-12-19 17:04:08</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Ensure steps before CONFIG_ERR_STATUS is correct.</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>4.35</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Alright, that was easy and quick.
+Now we need to brainstorm some more.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-12-19 17:13:26</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Understand theory of how to drive specific LED's on LED driver.</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>25.01</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>3.04</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>wENT and got coffee, but overall. Decent session. Focused, ect.
+Mainly due to my apps which is amazing.</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-12-19 17:45:59</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Determine CURRENT LIMIT for each type of LED</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>14.81</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Need to stick to my algorithm, and break goals down as they are too large and im procrastinating because of it.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-12-19 18:01:18</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>How to enable LED's.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>6.98</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>3.89</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>YAY FINISHED!!!! I wanna take a shit now. Lets do it fuck it!a</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-12-19 18:13:49</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Learn about setting PEAK CURRENT for both auto mode and individually controlled mode</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>13.30</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>4.54</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Finished the job. Good job!
+Algorithm complete!</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-12-19 18:56:38</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Read over datasheet to find anything that we may want to implement openly</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>13.56</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>13.30</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Er.. I have basicaly used all for MANUAL mode.</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-12-19 19:10:35</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Write comments in doxygen</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>20.01</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>26.07</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>165.52</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>didn't work. Didn't even transmit address, need to go back to yesterday.
+It is possible things just fried lol.
+Feel a little frustrated, going to deal with this failure by playing agames?</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-12-21 18:19:54</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>MEDITATE</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>43.45</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Erm fell asleep</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-12-25 09:33:37</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Watch the VIDEO and COPY all that you can. To learn about ICM20948</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>24.85</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>53.44</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Failed!!!! Maybe more coffee.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-12-25 10:57:23</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Lets IMMERSE ourselves in the BOREDOM of this IMU sensor!</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>43.29</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>18.66</t>
+        </is>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting to get distracted man. It doesn't matter what task but i'm running away.
+But what am I running away from?
+I believe it is from the sense of not knowing what i'm doing.
+It feels a bit big. Too big, and it scares me. So lets break it down
+that is our task.
+https://www.youtube.com/watch?v=p15H_ZQ4I1M
+.
+Lets take a deep breathe, and just be patient here. Let the unknown seep into our awareness and just be aware of it.
+Let the ideas from god flow into your mind. To allow you to solve thisproblem which will help not only yourself with meditation routine.
+But it will help a lot of different people.
+When your goal is too big. It becomes hard to move. It becomes easy to procrastinate. 
+Let go of your goals.
+Be very conscious of your thoughts, how you label things. When a challenge comes, like I realize I can burst write.
+Think of it as an oppportunity to learn. Not as a hindrance to our goal. "Now I have to do this"
+First I want to take a note as to what is going on in my mind at the moment.
+----------
+Session finished. God damn. This shit is interesting as heck.
+Lets practice getting better, try to improve in this weird place we are with our productivity. THis is an OPPORTUNITY TO learn and GROW about this weird human domain that exists within me.
+Try to be aware.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-12-25 12:04:26</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Lets IMMERSE ourselves in the BOREDOM of this IMU sensor!</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>45.01</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>13.31</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>18.05</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-12-25 13:39:51</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>STM32</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Lets IMMERSE ourselves in the BOREDOM of this IMU sensor!</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>40.60</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>13.31</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>